<commit_message>
Change TestObject folder structure and page naming convention to separate from functional tests
</commit_message>
<xml_diff>
--- a/InputFiles/Bento/Bento_StaticData.xlsx
+++ b/InputFiles/Bento/Bento_StaticData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/Bento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC85CC2-1085-5045-BB6D-92D216FFC60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60A5C97-D213-B84E-B27F-E53CE20795C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8840" yWindow="1260" windowWidth="36000" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Home_page" sheetId="1" r:id="rId1"/>
-    <sheet name="AboutBentoPage" sheetId="6" r:id="rId2"/>
-    <sheet name="AboutResourcesPage" sheetId="7" r:id="rId3"/>
+    <sheet name="V_HomePage" sheetId="1" r:id="rId1"/>
+    <sheet name="V_AboutBentoPage" sheetId="6" r:id="rId2"/>
+    <sheet name="V_AboutResourcesPage" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -592,8 +592,8 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A3" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -863,8 +863,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>